<commit_message>
fix bug, virtual addresses translator P addr has cells that is not updated. update prompt.
</commit_message>
<xml_diff>
--- a/virtual addresses translator.xlsx
+++ b/virtual addresses translator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8712f81eba3c7055/COMP/COMP2310/final/ANU-COMP2310-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="485" documentId="11_F25DC773A252ABDACC10487B411976065BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90014E28-2F3E-408E-9597-C2DFCD67B24E}"/>
+  <xr:revisionPtr revIDLastSave="503" documentId="11_F25DC773A252ABDACC10487B411976065BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0D73022-B210-4030-9085-ECBF225B065C}"/>
   <bookViews>
     <workbookView xWindow="-22046" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>V_addr_wide (bit)</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>CT</t>
+  </si>
+  <si>
+    <t>PPN (without 0x)</t>
+  </si>
+  <si>
+    <t>VPO / PPO</t>
   </si>
 </sst>
 </file>
@@ -247,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,7 +264,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,6 +343,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -605,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E4:E6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -629,131 +638,131 @@
         <v>29</v>
       </c>
       <c r="H1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(H1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" ref="H1:W1" si="0">_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(H1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
         <v>15</v>
       </c>
       <c r="I1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(I1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="J1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(J1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="K1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(K1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(L1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="M1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(M1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="N1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(N1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="O1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(O1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="P1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(P1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="Q1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(Q1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="R1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(R1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="S1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(S1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="T1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(T1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="U1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(U1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="V1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(V1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="W1" s="1">
-        <f>_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(W1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X1" s="1" t="str">
-        <f t="shared" ref="X1:AM1" si="0">_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(X1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
+        <f t="shared" ref="X1:AM1" si="1">_xlfn.LET(_xlpm.bit,$B$2-1-(COLUMN(X1)-COLUMN($H$1)),IF(_xlpm.bit &gt;= 0, _xlpm.bit,""))</f>
         <v/>
       </c>
       <c r="Y1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Z1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AA1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AB1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AC1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AD1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AE1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AF1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AG1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AH1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AI1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AJ1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AK1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AL1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AM1" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -771,63 +780,63 @@
         <v>13</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f t="shared" ref="H2:V2" si="1">IF(H1="","",IF(H1&lt;$B$10,"VPO","VPN"))</f>
+        <f t="shared" ref="H2:V2" si="2">IF(H1="","",IF(H1&lt;$B$10,"VPO","VPN"))</f>
         <v>VPN</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPN</v>
       </c>
       <c r="J2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPN</v>
       </c>
       <c r="K2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPN</v>
       </c>
       <c r="L2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPN</v>
       </c>
       <c r="M2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPN</v>
       </c>
       <c r="N2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPN</v>
       </c>
       <c r="O2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPO</v>
       </c>
       <c r="P2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPO</v>
       </c>
       <c r="Q2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPO</v>
       </c>
       <c r="R2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPO</v>
       </c>
       <c r="S2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPO</v>
       </c>
       <c r="T2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPO</v>
       </c>
       <c r="U2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPO</v>
       </c>
       <c r="V2" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>VPO</v>
       </c>
       <c r="W2" s="1" t="str">
@@ -835,67 +844,67 @@
         <v>VPO</v>
       </c>
       <c r="X2" s="1" t="str">
-        <f t="shared" ref="X2:AM2" si="2">IF(X1="","",IF(X1&lt;$B$10,"VPO","VPN"))</f>
+        <f t="shared" ref="X2:AM2" si="3">IF(X1="","",IF(X1&lt;$B$10,"VPO","VPN"))</f>
         <v/>
       </c>
       <c r="Y2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="Z2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AA2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AB2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AC2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AD2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AE2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AF2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AG2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AH2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AI2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AJ2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AK2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AL2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AM2" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -911,131 +920,131 @@
       </c>
       <c r="E3" s="5"/>
       <c r="H3" s="1" t="str">
-        <f>IF(H1="","",IF(H1&lt;$B$10,"VPO",IF(H1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" ref="H3:AM3" si="4">IF(H1="","",IF(H1&lt;$B$10,"VPO",IF(H1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
         <v>TLBT</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF(I1="","",IF(I1&lt;$B$10,"VPO",IF(I1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>TLBT</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f>IF(J1="","",IF(J1&lt;$B$10,"VPO",IF(J1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>TLBT</v>
       </c>
       <c r="K3" s="1" t="str">
-        <f>IF(K1="","",IF(K1&lt;$B$10,"VPO",IF(K1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>TLBT</v>
       </c>
       <c r="L3" s="1" t="str">
-        <f>IF(L1="","",IF(L1&lt;$B$10,"VPO",IF(L1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>TLBT</v>
       </c>
       <c r="M3" s="1" t="str">
-        <f>IF(M1="","",IF(M1&lt;$B$10,"VPO",IF(M1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>TLBT</v>
       </c>
       <c r="N3" s="1" t="str">
-        <f>IF(N1="","",IF(N1&lt;$B$10,"VPO",IF(N1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>TLBI</v>
       </c>
       <c r="O3" s="1" t="str">
-        <f>IF(O1="","",IF(O1&lt;$B$10,"VPO",IF(O1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="P3" s="1" t="str">
-        <f>IF(P1="","",IF(P1&lt;$B$10,"VPO",IF(P1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="Q3" s="1" t="str">
-        <f>IF(Q1="","",IF(Q1&lt;$B$10,"VPO",IF(Q1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="R3" s="1" t="str">
-        <f>IF(R1="","",IF(R1&lt;$B$10,"VPO",IF(R1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="S3" s="1" t="str">
-        <f>IF(S1="","",IF(S1&lt;$B$10,"VPO",IF(S1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="T3" s="1" t="str">
-        <f>IF(T1="","",IF(T1&lt;$B$10,"VPO",IF(T1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="U3" s="1" t="str">
-        <f>IF(U1="","",IF(U1&lt;$B$10,"VPO",IF(U1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="V3" s="1" t="str">
-        <f>IF(V1="","",IF(V1&lt;$B$10,"VPO",IF(V1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="W3" s="1" t="str">
-        <f>IF(W1="","",IF(W1&lt;$B$10,"VPO",IF(W1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v>VPO</v>
       </c>
       <c r="X3" s="1" t="str">
-        <f>IF(X1="","",IF(X1&lt;$B$10,"VPO",IF(X1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Y3" s="1" t="str">
-        <f>IF(Y1="","",IF(Y1&lt;$B$10,"VPO",IF(Y1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Z3" s="1" t="str">
-        <f>IF(Z1="","",IF(Z1&lt;$B$10,"VPO",IF(Z1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AA3" s="1" t="str">
-        <f>IF(AA1="","",IF(AA1&lt;$B$10,"VPO",IF(AA1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AB3" s="1" t="str">
-        <f>IF(AB1="","",IF(AB1&lt;$B$10,"VPO",IF(AB1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AC3" s="1" t="str">
-        <f>IF(AC1="","",IF(AC1&lt;$B$10,"VPO",IF(AC1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AD3" s="1" t="str">
-        <f>IF(AD1="","",IF(AD1&lt;$B$10,"VPO",IF(AD1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AE3" s="1" t="str">
-        <f>IF(AE1="","",IF(AE1&lt;$B$10,"VPO",IF(AE1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AF3" s="1" t="str">
-        <f>IF(AF1="","",IF(AF1&lt;$B$10,"VPO",IF(AF1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AG3" s="1" t="str">
-        <f>IF(AG1="","",IF(AG1&lt;$B$10,"VPO",IF(AG1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AH3" s="1" t="str">
-        <f>IF(AH1="","",IF(AH1&lt;$B$10,"VPO",IF(AH1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AI3" s="1" t="str">
-        <f>IF(AI1="","",IF(AI1&lt;$B$10,"VPO",IF(AI1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AJ3" s="1" t="str">
-        <f>IF(AJ1="","",IF(AJ1&lt;$B$10,"VPO",IF(AJ1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AK3" s="1" t="str">
-        <f>IF(AK1="","",IF(AK1&lt;$B$10,"VPO",IF(AK1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AL3" s="1" t="str">
-        <f>IF(AL1="","",IF(AL1&lt;$B$10,"VPO",IF(AL1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AM3" s="1" t="str">
-        <f>IF(AM1="","",IF(AM1&lt;$B$10,"VPO",IF(AM1&lt;($B$10+$B$12),"TLBI","TLBT")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1053,131 +1062,131 @@
         <v>2</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF(H1="","",MID($B$16,LEN($B$16)-H1,1))</f>
+        <f t="shared" ref="H4:AM4" si="5">IF(H1="","",MID($B$16,LEN($B$16)-H1,1))</f>
         <v>0</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF(I1="","",MID($B$16,LEN($B$16)-I1,1))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f>IF(J1="","",MID($B$16,LEN($B$16)-J1,1))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K4" s="1" t="str">
-        <f>IF(K1="","",MID($B$16,LEN($B$16)-K1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L4" s="1" t="str">
-        <f>IF(L1="","",MID($B$16,LEN($B$16)-L1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M4" s="1" t="str">
-        <f>IF(M1="","",MID($B$16,LEN($B$16)-M1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N4" s="1" t="str">
-        <f>IF(N1="","",MID($B$16,LEN($B$16)-N1,1))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O4" s="1" t="str">
-        <f>IF(O1="","",MID($B$16,LEN($B$16)-O1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P4" s="1" t="str">
-        <f>IF(P1="","",MID($B$16,LEN($B$16)-P1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q4" s="1" t="str">
-        <f>IF(Q1="","",MID($B$16,LEN($B$16)-Q1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R4" s="1" t="str">
-        <f>IF(R1="","",MID($B$16,LEN($B$16)-R1,1))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S4" s="1" t="str">
-        <f>IF(S1="","",MID($B$16,LEN($B$16)-S1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="T4" s="1" t="str">
-        <f>IF(T1="","",MID($B$16,LEN($B$16)-T1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U4" s="1" t="str">
-        <f>IF(U1="","",MID($B$16,LEN($B$16)-U1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="V4" s="1" t="str">
-        <f>IF(V1="","",MID($B$16,LEN($B$16)-V1,1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="W4" s="1" t="str">
-        <f>IF(W1="","",MID($B$16,LEN($B$16)-W1,1))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X4" s="1" t="str">
-        <f>IF(X1="","",MID($B$16,LEN($B$16)-X1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="Y4" s="1" t="str">
-        <f>IF(Y1="","",MID($B$16,LEN($B$16)-Y1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="Z4" s="1" t="str">
-        <f>IF(Z1="","",MID($B$16,LEN($B$16)-Z1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AA4" s="1" t="str">
-        <f>IF(AA1="","",MID($B$16,LEN($B$16)-AA1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AB4" s="1" t="str">
-        <f>IF(AB1="","",MID($B$16,LEN($B$16)-AB1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AC4" s="1" t="str">
-        <f>IF(AC1="","",MID($B$16,LEN($B$16)-AC1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AD4" s="1" t="str">
-        <f>IF(AD1="","",MID($B$16,LEN($B$16)-AD1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AE4" s="1" t="str">
-        <f>IF(AE1="","",MID($B$16,LEN($B$16)-AE1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AF4" s="1" t="str">
-        <f>IF(AF1="","",MID($B$16,LEN($B$16)-AF1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AG4" s="1" t="str">
-        <f>IF(AG1="","",MID($B$16,LEN($B$16)-AG1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AH4" s="1" t="str">
-        <f>IF(AH1="","",MID($B$16,LEN($B$16)-AH1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AI4" s="1" t="str">
-        <f>IF(AI1="","",MID($B$16,LEN($B$16)-AI1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AJ4" s="1" t="str">
-        <f>IF(AJ1="","",MID($B$16,LEN($B$16)-AJ1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AK4" s="1" t="str">
-        <f>IF(AK1="","",MID($B$16,LEN($B$16)-AK1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AL4" s="1" t="str">
-        <f>IF(AL1="","",MID($B$16,LEN($B$16)-AL1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AM4" s="1" t="str">
-        <f>IF(AM1="","",MID($B$16,LEN($B$16)-AM1,1))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -1206,131 +1215,131 @@
         <v>30</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF(H1="","",IF(H1&lt;$E$2,H1,""))</f>
+        <f t="shared" ref="H6:AM6" si="6">IF(H1="","",IF(H1&lt;$E$2,H1,""))</f>
         <v/>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF(I1="","",IF(I1&lt;$E$2,I1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J6" s="1" t="str">
-        <f>IF(J1="","",IF(J1&lt;$E$2,J1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="K6" s="1">
-        <f>IF(K1="","",IF(K1&lt;$E$2,K1,""))</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="L6" s="1">
-        <f>IF(L1="","",IF(L1&lt;$E$2,L1,""))</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="M6" s="1">
-        <f>IF(M1="","",IF(M1&lt;$E$2,M1,""))</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="N6" s="1">
-        <f>IF(N1="","",IF(N1&lt;$E$2,N1,""))</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="O6" s="1">
-        <f>IF(O1="","",IF(O1&lt;$E$2,O1,""))</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="P6" s="1">
-        <f>IF(P1="","",IF(P1&lt;$E$2,P1,""))</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="Q6" s="1">
-        <f>IF(Q1="","",IF(Q1&lt;$E$2,Q1,""))</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="R6" s="1">
-        <f>IF(R1="","",IF(R1&lt;$E$2,R1,""))</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="S6" s="1">
-        <f>IF(S1="","",IF(S1&lt;$E$2,S1,""))</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="T6" s="1">
-        <f>IF(T1="","",IF(T1&lt;$E$2,T1,""))</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="U6" s="1">
-        <f>IF(U1="","",IF(U1&lt;$E$2,U1,""))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="V6" s="1">
-        <f>IF(V1="","",IF(V1&lt;$E$2,V1,""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="W6" s="1">
-        <f>IF(W1="","",IF(W1&lt;$E$2,W1,""))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X6" s="1" t="str">
-        <f>IF(X1="","",IF(X1&lt;$E$2,X1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y6" s="1" t="str">
-        <f>IF(Y1="","",IF(Y1&lt;$E$2,Y1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z6" s="1" t="str">
-        <f>IF(Z1="","",IF(Z1&lt;$E$2,Z1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AA6" s="1" t="str">
-        <f>IF(AA1="","",IF(AA1&lt;$E$2,AA1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB6" s="1" t="str">
-        <f>IF(AB1="","",IF(AB1&lt;$E$2,AB1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AC6" s="1" t="str">
-        <f>IF(AC1="","",IF(AC1&lt;$E$2,AC1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD6" s="1" t="str">
-        <f>IF(AD1="","",IF(AD1&lt;$E$2,AD1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AE6" s="1" t="str">
-        <f>IF(AE1="","",IF(AE1&lt;$E$2,AE1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AF6" s="1" t="str">
-        <f>IF(AF1="","",IF(AF1&lt;$E$2,AF1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AG6" s="1" t="str">
-        <f>IF(AG1="","",IF(AG1&lt;$E$2,AG1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AH6" s="1" t="str">
-        <f>IF(AH1="","",IF(AH1&lt;$E$2,AH1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AI6" s="1" t="str">
-        <f>IF(AI1="","",IF(AI1&lt;$E$2,AI1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AJ6" s="1" t="str">
-        <f>IF(AJ1="","",IF(AJ1&lt;$E$2,AJ1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AK6" s="1" t="str">
-        <f>IF(AK1="","",IF(AK1&lt;$E$2,AK1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AL6" s="1" t="str">
-        <f>IF(AL1="","",IF(AL1&lt;$E$2,AL1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AM6" s="1" t="str">
-        <f>IF(AM1="","",IF(AM1&lt;$E$2,AM1,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -1342,63 +1351,63 @@
         <v>26</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f t="shared" ref="H7:V7" si="3">IF(H6="","",IF(H2="VPO","PPO","PPN"))</f>
+        <f t="shared" ref="H7:V7" si="7">IF(H6="","",IF(H2="VPO","PPO","PPN"))</f>
         <v/>
       </c>
       <c r="I7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPN</v>
       </c>
       <c r="L7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPN</v>
       </c>
       <c r="M7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPN</v>
       </c>
       <c r="N7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPN</v>
       </c>
       <c r="O7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPO</v>
       </c>
       <c r="P7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPO</v>
       </c>
       <c r="Q7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPO</v>
       </c>
       <c r="R7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPO</v>
       </c>
       <c r="S7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPO</v>
       </c>
       <c r="T7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPO</v>
       </c>
       <c r="U7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPO</v>
       </c>
       <c r="V7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>PPO</v>
       </c>
       <c r="W7" s="1" t="str">
@@ -1406,203 +1415,203 @@
         <v>PPO</v>
       </c>
       <c r="X7" s="1" t="str">
-        <f t="shared" ref="X7:AM7" si="4">IF(X6="","",IF(X2="VPO","PPO","PPN"))</f>
+        <f t="shared" ref="X7:AM7" si="8">IF(X6="","",IF(X2="VPO","PPO","PPN"))</f>
         <v/>
       </c>
       <c r="Y7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="Z7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AA7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AC7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AE7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AF7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AG7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AH7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AI7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AJ7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AK7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AL7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AM7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.45">
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF(H6="","",IF(H6&lt;$E$20,"CO",IF(H6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" ref="H8:AM8" si="9">IF(H6="","",IF(H6&lt;$E$20,"CO",IF(H6&lt;($E$20+$E$19),"CI","CT")))</f>
         <v/>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF(I6="","",IF(I6&lt;$E$20,"CO",IF(I6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J8" s="1" t="str">
-        <f>IF(J6="","",IF(J6&lt;$E$20,"CO",IF(J6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K8" s="1" t="str">
-        <f>IF(K6="","",IF(K6&lt;$E$20,"CO",IF(K6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CT</v>
       </c>
       <c r="L8" s="1" t="str">
-        <f>IF(L6="","",IF(L6&lt;$E$20,"CO",IF(L6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CT</v>
       </c>
       <c r="M8" s="1" t="str">
-        <f>IF(M6="","",IF(M6&lt;$E$20,"CO",IF(M6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CT</v>
       </c>
       <c r="N8" s="1" t="str">
-        <f>IF(N6="","",IF(N6&lt;$E$20,"CO",IF(N6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CT</v>
       </c>
       <c r="O8" s="1" t="str">
-        <f>IF(O6="","",IF(O6&lt;$E$20,"CO",IF(O6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CT</v>
       </c>
       <c r="P8" s="1" t="str">
-        <f>IF(P6="","",IF(P6&lt;$E$20,"CO",IF(P6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CT</v>
       </c>
       <c r="Q8" s="1" t="str">
-        <f>IF(Q6="","",IF(Q6&lt;$E$20,"CO",IF(Q6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CT</v>
       </c>
       <c r="R8" s="1" t="str">
-        <f>IF(R6="","",IF(R6&lt;$E$20,"CO",IF(R6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CT</v>
       </c>
       <c r="S8" s="1" t="str">
-        <f>IF(S6="","",IF(S6&lt;$E$20,"CO",IF(S6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CI</v>
       </c>
       <c r="T8" s="1" t="str">
-        <f>IF(T6="","",IF(T6&lt;$E$20,"CO",IF(T6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CI</v>
       </c>
       <c r="U8" s="1" t="str">
-        <f>IF(U6="","",IF(U6&lt;$E$20,"CO",IF(U6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CI</v>
       </c>
       <c r="V8" s="1" t="str">
-        <f>IF(V6="","",IF(V6&lt;$E$20,"CO",IF(V6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CO</v>
       </c>
       <c r="W8" s="1" t="str">
-        <f>IF(W6="","",IF(W6&lt;$E$20,"CO",IF(W6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v>CO</v>
       </c>
       <c r="X8" s="1" t="str">
-        <f>IF(X6="","",IF(X6&lt;$E$20,"CO",IF(X6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="Y8" s="1" t="str">
-        <f>IF(Y6="","",IF(Y6&lt;$E$20,"CO",IF(Y6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="Z8" s="1" t="str">
-        <f>IF(Z6="","",IF(Z6&lt;$E$20,"CO",IF(Z6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AA8" s="1" t="str">
-        <f>IF(AA6="","",IF(AA6&lt;$E$20,"CO",IF(AA6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB8" s="1" t="str">
-        <f>IF(AB6="","",IF(AB6&lt;$E$20,"CO",IF(AB6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AC8" s="1" t="str">
-        <f>IF(AC6="","",IF(AC6&lt;$E$20,"CO",IF(AC6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AD8" s="1" t="str">
-        <f>IF(AD6="","",IF(AD6&lt;$E$20,"CO",IF(AD6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AE8" s="1" t="str">
-        <f>IF(AE6="","",IF(AE6&lt;$E$20,"CO",IF(AE6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AF8" s="1" t="str">
-        <f>IF(AF6="","",IF(AF6&lt;$E$20,"CO",IF(AF6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AG8" s="1" t="str">
-        <f>IF(AG6="","",IF(AG6&lt;$E$20,"CO",IF(AG6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AH8" s="1" t="str">
-        <f>IF(AH6="","",IF(AH6&lt;$E$20,"CO",IF(AH6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AI8" s="1" t="str">
-        <f>IF(AI6="","",IF(AI6&lt;$E$20,"CO",IF(AI6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AJ8" s="1" t="str">
-        <f>IF(AJ6="","",IF(AJ6&lt;$E$20,"CO",IF(AJ6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AK8" s="1" t="str">
-        <f>IF(AK6="","",IF(AK6&lt;$E$20,"CO",IF(AK6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AL8" s="1" t="str">
-        <f>IF(AL6="","",IF(AL6&lt;$E$20,"CO",IF(AL6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AM8" s="1" t="str">
-        <f>IF(AM6="","",IF(AM6&lt;$E$20,"CO",IF(AM6&lt;($E$20+$E$19),"CI","CT")))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -1612,69 +1621,133 @@
       </c>
       <c r="B9" s="2"/>
       <c r="H9" s="1" t="str">
-        <f>IF(H6="","",MID(#REF!,#REF!-H6,1))</f>
+        <f t="shared" ref="H9:J9" si="10">IF(H6="","",MID($E$26,$E$11-H6,1))</f>
         <v/>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF(I6="","",MID(#REF!,#REF!-I6,1))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="J9" s="1" t="str">
-        <f>IF(J6="","",MID(#REF!,#REF!-J6,1))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="K9" s="1" t="str">
-        <f t="shared" ref="K9:V9" si="5">IF(K6="","",MID($E$26,$E$11-K6,1))</f>
+        <f t="shared" ref="K9:V9" si="11">IF(K6="","",MID($E$26,$E$11-K6,1))</f>
         <v>0</v>
       </c>
       <c r="L9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="P9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="Q9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="T9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="U9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="V9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="W9" s="1" t="str">
         <f>IF(W6="","",MID($E$26,$E$11-W6,1))</f>
         <v>0</v>
       </c>
+      <c r="X9" s="1" t="str">
+        <f t="shared" ref="X9:AM9" si="12">IF(X6="","",MID($E$26,$E$11-X6,1))</f>
+        <v/>
+      </c>
+      <c r="Y9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="Z9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AA9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AB9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AC9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AD9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AE9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AF9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AG9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AH9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AI9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AJ9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AK9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AL9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AM9" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
@@ -1830,14 +1903,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="3" t="str">
         <f>LEFT(RIGHT(B16,B10+B11),B11)</f>
         <v>0001110</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E21" s="3">
@@ -1857,7 +1930,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B24" s="3" t="str" cm="1">
         <f t="array" ref="B24">_xlfn.LET(_xlpm.x,B18, _xlpm.bi, IF(MOD(LEN(_xlpm.x),4)=0,_xlpm.x,_xlfn.CONCAT(REPT("0",4-MOD(LEN(_xlpm.x),4)), _xlpm.x)), _xlfn.TEXTJOIN("",TRUE,BIN2HEX(MID(_xlpm.bi,_xlfn.SEQUENCE(LEN(_xlpm.bi)/4,,,4),4),1)))</f>
@@ -1904,14 +1977,14 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="3" t="str" cm="1">
         <f t="array" ref="B27">_xlfn.LET(_xlpm.x,B21, _xlpm.bi, IF(MOD(LEN(_xlpm.x),4)=0,_xlpm.x,_xlfn.CONCAT(REPT("0",4-MOD(LEN(_xlpm.x),4)), _xlpm.x)), _xlfn.TEXTJOIN("",TRUE,BIN2HEX(MID(_xlpm.bi,_xlfn.SEQUENCE(LEN(_xlpm.bi)/4,,,4),4),1)))</f>
         <v>0E</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E27" s="3" t="str">
@@ -1920,7 +1993,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E28" s="3" t="str">
@@ -1929,7 +2002,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="3" t="str">

</xml_diff>

<commit_message>
fix virtual addresses translator, addr is set to be TEXT formate
</commit_message>
<xml_diff>
--- a/virtual addresses translator.xlsx
+++ b/virtual addresses translator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8712f81eba3c7055/COMP/COMP2310/final/ANU-COMP2310-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="503" documentId="11_F25DC773A252ABDACC10487B411976065BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0D73022-B210-4030-9085-ECBF225B065C}"/>
+  <xr:revisionPtr revIDLastSave="505" documentId="11_F25DC773A252ABDACC10487B411976065BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69FA7CC6-47D5-4BF5-8AB8-79136FFFBCAE}"/>
   <bookViews>
-    <workbookView xWindow="-22046" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="16395" windowHeight="28276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -264,6 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +616,7 @@
   <dimension ref="A1:AM35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1347,7 +1348,7 @@
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="1" t="str">
@@ -1483,7 +1484,7 @@
       <c r="D8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="6">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="str">

</xml_diff>